<commit_message>
Documentación y BD Inicial
Documentación Final de la Base de Datos y Base de Datos Inicial
</commit_message>
<xml_diff>
--- a/Docs/DB CSAdmin.xlsx
+++ b/Docs/DB CSAdmin.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="77">
   <si>
     <t>Clave</t>
   </si>
@@ -33,15 +33,6 @@
     <t>CK</t>
   </si>
   <si>
-    <t>Texto</t>
-  </si>
-  <si>
-    <t>Fecha</t>
-  </si>
-  <si>
-    <t>Numerico</t>
-  </si>
-  <si>
     <t>FK</t>
   </si>
   <si>
@@ -87,9 +78,6 @@
     <t>FuncionId</t>
   </si>
   <si>
-    <t>TelPersonas</t>
-  </si>
-  <si>
     <t>IdPersona</t>
   </si>
   <si>
@@ -144,30 +132,15 @@
     <t>Localidad</t>
   </si>
   <si>
-    <t>Sede</t>
-  </si>
-  <si>
     <t>Coordinador</t>
   </si>
   <si>
-    <t>????</t>
-  </si>
-  <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>Cargo</t>
   </si>
   <si>
     <t>Condicion</t>
   </si>
   <si>
-    <t>Condicioin</t>
-  </si>
-  <si>
-    <t>Contrato</t>
-  </si>
-  <si>
     <t>CargoId</t>
   </si>
   <si>
@@ -178,23 +151,112 @@
   </si>
   <si>
     <t>FechaInicio</t>
+  </si>
+  <si>
+    <t>Baja</t>
+  </si>
+  <si>
+    <t>CargoAbrev</t>
+  </si>
+  <si>
+    <t>CondicionAbrev</t>
+  </si>
+  <si>
+    <t>Origen</t>
+  </si>
+  <si>
+    <t>Horas</t>
+  </si>
+  <si>
+    <t>Observacion</t>
+  </si>
+  <si>
+    <t>Afectado</t>
+  </si>
+  <si>
+    <t>Contratos</t>
+  </si>
+  <si>
+    <t>Funciones</t>
+  </si>
+  <si>
+    <t>SituacionesProfesionales</t>
+  </si>
+  <si>
+    <t>datetime(8)</t>
+  </si>
+  <si>
+    <t>bit(1)</t>
+  </si>
+  <si>
+    <t>nvarchar(60)</t>
+  </si>
+  <si>
+    <t>nvarchar(8)</t>
+  </si>
+  <si>
+    <t>nvarchar(10)</t>
+  </si>
+  <si>
+    <t>nvarchar(20)</t>
+  </si>
+  <si>
+    <t>tinyint</t>
+  </si>
+  <si>
+    <t>nvarchar(100)</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>nvarchar(40)</t>
+  </si>
+  <si>
+    <t>nvarchar(30)</t>
+  </si>
+  <si>
+    <t>numeric(12,0)</t>
+  </si>
+  <si>
+    <t>nvarchar(50)</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>nvarchar(140)</t>
+  </si>
+  <si>
+    <t>bit</t>
+  </si>
+  <si>
+    <t>numeric(9,0)</t>
+  </si>
+  <si>
+    <t>numeric(11,0)</t>
+  </si>
+  <si>
+    <t>PersonasTel</t>
+  </si>
+  <si>
+    <t>nchar(2)</t>
+  </si>
+  <si>
+    <t>nvarchar(3)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -263,18 +325,18 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -571,21 +633,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H80"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -613,7 +676,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -622,22 +685,22 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
@@ -645,79 +708,83 @@
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>7</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="B13" s="3"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -736,7 +803,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="7" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -745,7 +812,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
@@ -753,33 +820,33 @@
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -798,7 +865,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -807,7 +874,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
@@ -815,44 +882,44 @@
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="3" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -871,7 +938,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -880,22 +947,22 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3" t="s">
@@ -903,40 +970,42 @@
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -955,7 +1024,7 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -964,7 +1033,7 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
@@ -972,427 +1041,448 @@
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>45</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10" t="s">
-        <v>5</v>
+      <c r="A41" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" s="3"/>
+      <c r="A42" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B43" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="3" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
+      <c r="C44" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="9"/>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
       <c r="F46" s="9"/>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="9"/>
+      <c r="A47" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="A48" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B49" s="3"/>
-      <c r="C49" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
       <c r="E49" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="11"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="10"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="7" t="s">
+    <row r="52" spans="1:7">
+      <c r="A52" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="B53" s="3"/>
+      <c r="C53" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G53" s="9"/>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" s="3" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="B54" s="3"/>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="6"/>
-      <c r="B56" s="6"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="6"/>
+        <v>58</v>
+      </c>
+      <c r="G55" s="9"/>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G56" s="9"/>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="10"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3" t="s">
+    <row r="58" spans="1:7">
+      <c r="A58" s="6"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="3" t="s">
+      <c r="D60" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="6"/>
-      <c r="B61" s="6"/>
-      <c r="C61" s="6"/>
-      <c r="D61" s="6"/>
-      <c r="E61" s="6"/>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="6"/>
-      <c r="B62" s="6"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="6"/>
-      <c r="E62" s="6"/>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
-      <c r="A65" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="B65" s="3"/>
-      <c r="C65" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
+      <c r="C66" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
+      <c r="C67" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="D67" s="3"/>
       <c r="E67" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="B68" s="3"/>
       <c r="C68" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H68" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="B69" s="3"/>
       <c r="C69" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="B70" s="3"/>
-      <c r="C70" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8">
-      <c r="A71" s="6"/>
-      <c r="B71" s="6"/>
-      <c r="C71" s="6"/>
-      <c r="D71" s="6"/>
-      <c r="E71" s="6"/>
-    </row>
-    <row r="72" spans="1:8">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72" s="6"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
       <c r="D72" s="6"/>
       <c r="E72" s="6"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:5">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
       <c r="E73" s="6"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:5">
       <c r="A74" s="6"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
       <c r="E74" s="6"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:5">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
       <c r="E75" s="6"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:5">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
       <c r="D76" s="6"/>
       <c r="E76" s="6"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:5">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
       <c r="E77" s="6"/>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:5">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
       <c r="E78" s="6"/>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:5">
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
       <c r="D79" s="6"/>
       <c r="E79" s="6"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:5">
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
       <c r="E80" s="6"/>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="6"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Migración de SQL CE a SQL Server Express
Debido a cambio en los requerimientos se migró la base de datos de SQL
Compact Edition a SQL Server 2008 Express.
</commit_message>
<xml_diff>
--- a/Docs/DB CSAdmin.xlsx
+++ b/Docs/DB CSAdmin.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="75">
   <si>
     <t>Clave</t>
   </si>
@@ -180,18 +180,9 @@
     <t>SituacionesProfesionales</t>
   </si>
   <si>
-    <t>datetime(8)</t>
-  </si>
-  <si>
-    <t>bit(1)</t>
-  </si>
-  <si>
     <t>nvarchar(60)</t>
   </si>
   <si>
-    <t>nvarchar(8)</t>
-  </si>
-  <si>
     <t>nvarchar(10)</t>
   </si>
   <si>
@@ -222,9 +213,6 @@
     <t>int</t>
   </si>
   <si>
-    <t>datetime</t>
-  </si>
-  <si>
     <t>nvarchar(140)</t>
   </si>
   <si>
@@ -243,10 +231,16 @@
     <t>nchar(2)</t>
   </si>
   <si>
-    <t>nvarchar(3)</t>
-  </si>
-  <si>
     <t>Contra</t>
+  </si>
+  <si>
+    <t>nchar(3)</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>nchar(8)</t>
   </si>
 </sst>
 </file>
@@ -296,7 +290,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -319,6 +313,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -332,13 +339,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -647,13 +654,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1"/>
@@ -695,7 +702,7 @@
         <v>13</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -708,7 +715,7 @@
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -716,7 +723,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>4</v>
@@ -725,7 +732,7 @@
         <v>29</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -736,7 +743,7 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -747,7 +754,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -755,12 +762,12 @@
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -768,12 +775,12 @@
         <v>16</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -784,7 +791,7 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -803,7 +810,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -820,7 +827,7 @@
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -835,7 +842,7 @@
         <v>22</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -846,7 +853,7 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -874,52 +881,52 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="8"/>
+      <c r="D23" s="3"/>
       <c r="E23" s="3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3" t="s">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="C24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="12"/>
       <c r="E24" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="3"/>
-      <c r="C26" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E26" s="3" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -957,7 +964,7 @@
         <v>13</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -970,7 +977,7 @@
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -981,7 +988,7 @@
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -992,7 +999,7 @@
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1000,12 +1007,12 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1041,7 +1048,7 @@
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1052,7 +1059,7 @@
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1063,7 +1070,7 @@
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1071,25 +1078,25 @@
         <v>16</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1097,12 +1104,12 @@
         <v>10</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1115,7 +1122,7 @@
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1124,7 +1131,7 @@
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
-      <c r="F45" s="9"/>
+      <c r="F45" s="8"/>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="6"/>
@@ -1132,7 +1139,7 @@
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
-      <c r="F46" s="9"/>
+      <c r="F46" s="8"/>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="7" t="s">
@@ -1153,7 +1160,7 @@
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1164,11 +1171,11 @@
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="10"/>
+      <c r="A50" s="9"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
@@ -1182,7 +1189,7 @@
       <c r="E51" s="6"/>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="11" t="s">
+      <c r="A52" s="10" t="s">
         <v>53</v>
       </c>
       <c r="B52" s="5"/>
@@ -1200,9 +1207,9 @@
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G53" s="9"/>
+        <v>74</v>
+      </c>
+      <c r="G53" s="8"/>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="3" t="s">
@@ -1212,7 +1219,7 @@
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1225,9 +1232,9 @@
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G55" s="9"/>
+        <v>74</v>
+      </c>
+      <c r="G55" s="8"/>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="3" t="s">
@@ -1237,12 +1244,12 @@
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G56" s="9"/>
+        <v>63</v>
+      </c>
+      <c r="G56" s="8"/>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="10"/>
+      <c r="A57" s="9"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
@@ -1276,7 +1283,7 @@
         <v>13</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -1289,7 +1296,7 @@
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -1300,7 +1307,7 @@
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -1308,12 +1315,12 @@
         <v>42</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -1324,7 +1331,7 @@
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1335,7 +1342,7 @@
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1348,7 +1355,7 @@
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1361,7 +1368,7 @@
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="3" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -1374,7 +1381,7 @@
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1387,7 +1394,7 @@
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1398,7 +1405,7 @@
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -1406,12 +1413,12 @@
         <v>49</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
       <c r="E71" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="72" spans="1:5">

</xml_diff>

<commit_message>
Se agregó tabla Localidades a BD
Se agregó una tabla Localidades a la BD y se relaciono con la tabla
Equipos.
</commit_message>
<xml_diff>
--- a/Docs/DB CSAdmin.xlsx
+++ b/Docs/DB CSAdmin.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
@@ -11,12 +11,12 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="77">
   <si>
     <t>Clave</t>
   </si>
@@ -241,6 +241,12 @@
   </si>
   <si>
     <t>nchar(8)</t>
+  </si>
+  <si>
+    <t>LocalidadId</t>
+  </si>
+  <si>
+    <t>Localidades</t>
   </si>
 </sst>
 </file>
@@ -342,10 +348,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -642,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -654,13 +660,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1"/>
@@ -900,7 +906,7 @@
       <c r="C24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="12"/>
+      <c r="D24" s="11"/>
       <c r="E24" s="3" t="s">
         <v>56</v>
       </c>
@@ -1064,13 +1070,15 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="3" t="s">
-        <v>36</v>
+        <v>75</v>
       </c>
       <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
+      <c r="C40" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1429,25 +1437,39 @@
       <c r="E72" s="6"/>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="6"/>
-      <c r="B73" s="6"/>
-      <c r="C73" s="6"/>
-      <c r="D73" s="6"/>
-      <c r="E73" s="6"/>
+      <c r="A73" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
     </row>
     <row r="74" spans="1:5">
-      <c r="A74" s="6"/>
-      <c r="B74" s="6"/>
-      <c r="C74" s="6"/>
-      <c r="D74" s="6"/>
-      <c r="E74" s="6"/>
+      <c r="A74" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="75" spans="1:5">
-      <c r="A75" s="6"/>
-      <c r="B75" s="6"/>
-      <c r="C75" s="6"/>
-      <c r="D75" s="6"/>
-      <c r="E75" s="6"/>
+      <c r="A75" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="6"/>

</xml_diff>